<commit_message>
Fixed the file name issue
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18530" windowHeight="7070" tabRatio="500"/>
+    <workbookView windowWidth="22188" windowHeight="9252" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -163,7 +163,7 @@
     <t>Running Organisation Suite</t>
   </si>
   <si>
-    <t>Organisation</t>
+    <t>Organization</t>
   </si>
   <si>
     <t>Organisation.data</t>
@@ -175,9 +175,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="30">
     <font>
@@ -254,15 +254,24 @@
       <charset val="134"/>
     </font>
     <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -276,17 +285,27 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -298,6 +317,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -306,21 +332,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -329,14 +340,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -345,38 +348,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -390,13 +363,40 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="35">
     <fill>
@@ -419,13 +419,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -437,169 +599,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -739,11 +739,50 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -759,21 +798,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -796,23 +820,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -827,158 +836,149 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="18" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1044,11 +1044,11 @@
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="7" fillId="3" borderId="8" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top"/>
       <protection locked="0"/>
     </xf>
@@ -1133,52 +1133,52 @@
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="40% - Accent1" xfId="1" builtinId="31"/>
-    <cellStyle name="Comma" xfId="2" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="3" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="4" builtinId="7"/>
-    <cellStyle name="Currency" xfId="5" builtinId="4"/>
-    <cellStyle name="Percent" xfId="6" builtinId="5"/>
-    <cellStyle name="Hyperlink" xfId="7" builtinId="8"/>
-    <cellStyle name="60% - Accent4" xfId="8" builtinId="44"/>
-    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9"/>
-    <cellStyle name="Check Cell" xfId="10" builtinId="23"/>
-    <cellStyle name="Heading 2" xfId="11" builtinId="17"/>
-    <cellStyle name="Note" xfId="12" builtinId="10"/>
-    <cellStyle name="40% - Accent3" xfId="13" builtinId="39"/>
-    <cellStyle name="Warning Text" xfId="14" builtinId="11"/>
-    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
-    <cellStyle name="Title" xfId="16" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="17" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="18" builtinId="16"/>
-    <cellStyle name="Heading 3" xfId="19" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="20" builtinId="19"/>
-    <cellStyle name="Input" xfId="21" builtinId="20"/>
-    <cellStyle name="60% - Accent3" xfId="22" builtinId="40"/>
-    <cellStyle name="Good" xfId="23" builtinId="26"/>
-    <cellStyle name="Output" xfId="24" builtinId="21"/>
-    <cellStyle name="20% - Accent1" xfId="25" builtinId="30"/>
-    <cellStyle name="Calculation" xfId="26" builtinId="22"/>
-    <cellStyle name="Linked Cell" xfId="27" builtinId="24"/>
-    <cellStyle name="Total" xfId="28" builtinId="25"/>
-    <cellStyle name="Bad" xfId="29" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="30" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="31" builtinId="29"/>
-    <cellStyle name="20% - Accent5" xfId="32" builtinId="46"/>
-    <cellStyle name="60% - Accent1" xfId="33" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="34" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="35" builtinId="34"/>
-    <cellStyle name="20% - Accent6" xfId="36" builtinId="50"/>
-    <cellStyle name="60% - Accent2" xfId="37" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="38" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="39" builtinId="38"/>
-    <cellStyle name="Accent4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="42" builtinId="43"/>
-    <cellStyle name="Accent5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - Accent5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="45" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="46" builtinId="49"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
     <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
     <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
@@ -1524,10 +1524,10 @@
   <dimension ref="A1:M50"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="38.8333333333333" style="3" customWidth="1"/>
     <col min="2" max="2" width="25" style="4" customWidth="1"/>

</xml_diff>

<commit_message>
Made changes in the plan file
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9287" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -30,7 +30,20 @@
     <definedName name="webcookie">'[1]#system'!$O$2:$O$8</definedName>
     <definedName name="ws">'[1]#system'!$P$2:$P$15</definedName>
   </definedNames>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -184,7 +197,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
@@ -1569,11 +1582,11 @@
   <sheetPr/>
   <dimension ref="A1:M49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="47.9" style="3" customWidth="1"/>
     <col min="2" max="2" width="25" style="4" customWidth="1"/>
@@ -1735,10 +1748,10 @@
       <c r="M6" s="41"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A7" s="28" t="s">
+      <c r="A7" s="31" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="23" t="s">
+      <c r="B7" s="32" t="s">
         <v>25</v>
       </c>
       <c r="C7" s="23"/>
@@ -1760,10 +1773,10 @@
       <c r="M7" s="41"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="23" t="s">
+      <c r="B8" s="32" t="s">
         <v>27</v>
       </c>
       <c r="C8" s="23"/>
@@ -1785,10 +1798,10 @@
       <c r="M8" s="41"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A9" s="28" t="s">
+      <c r="A9" s="31" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="32" t="s">
         <v>29</v>
       </c>
       <c r="C9" s="23"/>
@@ -1810,10 +1823,10 @@
       <c r="M9" s="41"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A10" s="28" t="s">
+      <c r="A10" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="32" t="s">
         <v>31</v>
       </c>
       <c r="C10" s="23"/>
@@ -1835,10 +1848,10 @@
       <c r="M10" s="41"/>
     </row>
     <row r="11" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A11" s="28" t="s">
+      <c r="A11" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="32" t="s">
         <v>33</v>
       </c>
       <c r="C11" s="23"/>
@@ -1860,10 +1873,10 @@
       <c r="M11" s="41"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="31" t="s">
         <v>34</v>
       </c>
-      <c r="B12" s="23" t="s">
+      <c r="B12" s="32" t="s">
         <v>35</v>
       </c>
       <c r="C12" s="23"/>
@@ -1885,10 +1898,10 @@
       <c r="M12" s="41"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A13" s="28" t="s">
+      <c r="A13" s="31" t="s">
         <v>36</v>
       </c>
-      <c r="B13" s="23" t="s">
+      <c r="B13" s="32" t="s">
         <v>37</v>
       </c>
       <c r="C13" s="23"/>
@@ -1910,10 +1923,10 @@
       <c r="M13" s="41"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A14" s="28" t="s">
+      <c r="A14" s="31" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="32" t="s">
         <v>39</v>
       </c>
       <c r="C14" s="24"/>
@@ -1935,10 +1948,10 @@
       <c r="M14" s="41"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A15" s="28" t="s">
+      <c r="A15" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="32" t="s">
         <v>41</v>
       </c>
       <c r="C15" s="23"/>

</xml_diff>

<commit_message>
modified the test plan
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9264" tabRatio="500"/>
+    <workbookView windowWidth="18350" windowHeight="6920" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Test Plan" sheetId="2" r:id="rId1"/>
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
   <si>
     <t>summary</t>
   </si>
@@ -104,10 +104,10 @@
     <t>reason</t>
   </si>
   <si>
-    <t>GKUser Core API Test Suite</t>
-  </si>
-  <si>
-    <t>GKUser</t>
+    <t>Customer and Supplier Core API Test Suite</t>
+  </si>
+  <si>
+    <t>CustomerandSupplier</t>
   </si>
   <si>
     <t>yes</t>
@@ -116,82 +116,16 @@
     <t>no</t>
   </si>
   <si>
-    <t>GNUKhata Core API Test Suite</t>
-  </si>
-  <si>
-    <t>GNUKhata</t>
-  </si>
-  <si>
-    <t>Accounts Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Account</t>
-  </si>
-  <si>
-    <t>AuditLogs Core API Test Suite</t>
-  </si>
-  <si>
-    <t>AuditLogs</t>
-  </si>
-  <si>
-    <t>Customer and Supplier Core API Test Suite</t>
-  </si>
-  <si>
-    <t>CustomerandSupplier</t>
-  </si>
-  <si>
-    <t>Invite Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Invite</t>
-  </si>
-  <si>
-    <t>Invoice Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Invoice</t>
-  </si>
-  <si>
     <t>Product Core API Test Suite</t>
   </si>
   <si>
     <t>Product</t>
   </si>
   <si>
-    <t>Reports Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Reports</t>
-  </si>
-  <si>
     <t>Tax Core API Test Suite</t>
   </si>
   <si>
     <t>Tax</t>
-  </si>
-  <si>
-    <t>Deliverynote  Core API Test Suite</t>
-  </si>
-  <si>
-    <t>DeliveryNote</t>
-  </si>
-  <si>
-    <t>Export - Import  Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Export-Import</t>
-  </si>
-  <si>
-    <t>CloseBook and RollOver Core API Test Suite</t>
-  </si>
-  <si>
-    <t>CloseBook-RollOver</t>
-  </si>
-  <si>
-    <t>Organization Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Organization</t>
   </si>
 </sst>
 </file>
@@ -204,7 +138,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="30">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -261,21 +195,6 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Tahoma"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <strike/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Consolas"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Consolas"/>
       <charset val="134"/>
@@ -644,7 +563,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -770,15 +689,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -894,135 +804,135 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="5" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="6" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="18" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1119,41 +1029,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1580,13 +1467,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M49"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
   <cols>
     <col min="1" max="1" width="47.9" style="3" customWidth="1"/>
     <col min="2" max="2" width="25" style="4" customWidth="1"/>
@@ -1618,13 +1505,13 @@
       <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="37"/>
-      <c r="J1" s="38"/>
+      <c r="I1" s="31"/>
+      <c r="J1" s="32"/>
       <c r="K1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="39"/>
-      <c r="M1" s="40"/>
+      <c r="L1" s="33"/>
+      <c r="M1" s="34"/>
     </row>
     <row r="2" ht="147" customHeight="1" spans="1:13">
       <c r="A2" s="16" t="s">
@@ -1638,10 +1525,10 @@
       <c r="G2" s="20"/>
       <c r="H2" s="21"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="41"/>
-      <c r="K2" s="42"/>
-      <c r="L2" s="43"/>
-      <c r="M2" s="44"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="37"/>
+      <c r="M2" s="38"/>
     </row>
     <row r="3" ht="10" customHeight="1" spans="1:13">
       <c r="A3" s="22"/>
@@ -1653,10 +1540,10 @@
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="41"/>
-      <c r="K3" s="45"/>
-      <c r="L3" s="46"/>
-      <c r="M3" s="41"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="40"/>
+      <c r="M3" s="35"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="20" customHeight="1" spans="1:13">
       <c r="A4" s="26" t="s">
@@ -1686,8 +1573,8 @@
       <c r="I4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="41"/>
-      <c r="K4" s="47" t="s">
+      <c r="J4" s="35"/>
+      <c r="K4" s="41" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="26" t="s">
@@ -1706,8 +1593,8 @@
       </c>
       <c r="C5" s="23"/>
       <c r="D5" s="24"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="30" t="s">
+      <c r="E5" s="24"/>
+      <c r="F5" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G5" s="25" t="s">
@@ -1717,10 +1604,10 @@
         <v>21</v>
       </c>
       <c r="I5" s="23"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="46"/>
-      <c r="M5" s="41"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="39"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="35"/>
     </row>
     <row r="6" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A6" s="28" t="s">
@@ -1731,8 +1618,8 @@
       </c>
       <c r="C6" s="23"/>
       <c r="D6" s="24"/>
-      <c r="E6" s="29"/>
-      <c r="F6" s="30" t="s">
+      <c r="E6" s="24"/>
+      <c r="F6" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G6" s="25" t="s">
@@ -1742,22 +1629,22 @@
         <v>21</v>
       </c>
       <c r="I6" s="23"/>
-      <c r="J6" s="41"/>
-      <c r="K6" s="45"/>
-      <c r="L6" s="46"/>
-      <c r="M6" s="41"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="39"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="35"/>
     </row>
     <row r="7" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="32" t="s">
+      <c r="B7" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="23"/>
+      <c r="C7" s="24"/>
       <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="30" t="s">
+      <c r="E7" s="23"/>
+      <c r="F7" s="29" t="s">
         <v>20</v>
       </c>
       <c r="G7" s="25" t="s">
@@ -1767,285 +1654,175 @@
         <v>21</v>
       </c>
       <c r="I7" s="23"/>
-      <c r="J7" s="41"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="46"/>
-      <c r="M7" s="41"/>
+      <c r="J7" s="35"/>
+      <c r="K7" s="39"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="35"/>
     </row>
     <row r="8" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A8" s="31" t="s">
-        <v>26</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>27</v>
-      </c>
-      <c r="C8" s="23"/>
+      <c r="A8" s="22"/>
+      <c r="B8" s="23"/>
+      <c r="C8" s="24"/>
       <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
-      <c r="F8" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E8" s="23"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="25"/>
       <c r="I8" s="23"/>
-      <c r="J8" s="41"/>
-      <c r="K8" s="45"/>
-      <c r="L8" s="46"/>
-      <c r="M8" s="41"/>
+      <c r="J8" s="35"/>
+      <c r="K8" s="39"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="35"/>
     </row>
     <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A9" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="B9" s="23" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="23"/>
+      <c r="A9" s="22"/>
+      <c r="B9" s="23"/>
+      <c r="C9" s="24"/>
       <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E9" s="23"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="23"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="45"/>
-      <c r="L9" s="46"/>
-      <c r="M9" s="41"/>
+      <c r="J9" s="35"/>
+      <c r="K9" s="39"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="35"/>
     </row>
     <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A10" s="31" t="s">
-        <v>30</v>
-      </c>
-      <c r="B10" s="32" t="s">
-        <v>31</v>
-      </c>
-      <c r="C10" s="23"/>
+      <c r="A10" s="22"/>
+      <c r="B10" s="23"/>
+      <c r="C10" s="24"/>
       <c r="D10" s="24"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G10" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H10" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E10" s="23"/>
+      <c r="F10" s="25"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
       <c r="I10" s="23"/>
-      <c r="J10" s="41"/>
-      <c r="K10" s="45"/>
-      <c r="L10" s="46"/>
-      <c r="M10" s="41"/>
+      <c r="J10" s="35"/>
+      <c r="K10" s="39"/>
+      <c r="L10" s="40"/>
+      <c r="M10" s="35"/>
     </row>
     <row r="11" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A11" s="31" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C11" s="23"/>
+      <c r="A11" s="22"/>
+      <c r="B11" s="23"/>
+      <c r="C11" s="24"/>
       <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H11" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E11" s="23"/>
+      <c r="F11" s="25"/>
+      <c r="G11" s="25"/>
+      <c r="H11" s="25"/>
       <c r="I11" s="23"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="45"/>
-      <c r="L11" s="46"/>
-      <c r="M11" s="41"/>
+      <c r="J11" s="35"/>
+      <c r="K11" s="39"/>
+      <c r="L11" s="40"/>
+      <c r="M11" s="35"/>
     </row>
     <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A12" s="28" t="s">
-        <v>34</v>
-      </c>
-      <c r="B12" s="23" t="s">
-        <v>35</v>
-      </c>
-      <c r="C12" s="23"/>
+      <c r="A12" s="22"/>
+      <c r="B12" s="23"/>
+      <c r="C12" s="24"/>
       <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G12" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H12" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E12" s="23"/>
+      <c r="F12" s="25"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="25"/>
       <c r="I12" s="23"/>
-      <c r="J12" s="41"/>
-      <c r="K12" s="45"/>
-      <c r="L12" s="46"/>
-      <c r="M12" s="41"/>
+      <c r="J12" s="35"/>
+      <c r="K12" s="39"/>
+      <c r="L12" s="40"/>
+      <c r="M12" s="35"/>
     </row>
     <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B13" s="32" t="s">
-        <v>37</v>
-      </c>
-      <c r="C13" s="23"/>
+      <c r="A13" s="22"/>
+      <c r="B13" s="23"/>
+      <c r="C13" s="24"/>
       <c r="D13" s="24"/>
       <c r="E13" s="23"/>
-      <c r="F13" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G13" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H13" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="F13" s="25"/>
+      <c r="G13" s="25"/>
+      <c r="H13" s="25"/>
       <c r="I13" s="23"/>
-      <c r="J13" s="41"/>
-      <c r="K13" s="45"/>
-      <c r="L13" s="46"/>
-      <c r="M13" s="41"/>
+      <c r="J13" s="35"/>
+      <c r="K13" s="39"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="35"/>
     </row>
     <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A14" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="B14" s="23" t="s">
-        <v>39</v>
-      </c>
+      <c r="A14" s="22"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="24"/>
       <c r="D14" s="24"/>
       <c r="E14" s="23"/>
-      <c r="F14" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H14" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="F14" s="25"/>
+      <c r="G14" s="25"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="23"/>
-      <c r="J14" s="41"/>
-      <c r="K14" s="45"/>
-      <c r="L14" s="46"/>
-      <c r="M14" s="41"/>
+      <c r="J14" s="35"/>
+      <c r="K14" s="39"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="35"/>
     </row>
     <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A15" s="31" t="s">
-        <v>40</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>41</v>
-      </c>
-      <c r="C15" s="23"/>
+      <c r="A15" s="22"/>
+      <c r="B15" s="23"/>
+      <c r="C15" s="24"/>
       <c r="D15" s="24"/>
-      <c r="E15" s="24"/>
-      <c r="F15" s="30" t="s">
-        <v>20</v>
-      </c>
-      <c r="G15" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H15" s="25" t="s">
-        <v>21</v>
-      </c>
+      <c r="E15" s="23"/>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="25"/>
       <c r="I15" s="23"/>
-      <c r="J15" s="41"/>
-      <c r="K15" s="45"/>
-      <c r="L15" s="46"/>
-      <c r="M15" s="41"/>
+      <c r="J15" s="35"/>
+      <c r="K15" s="39"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="35"/>
     </row>
     <row r="16" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A16" s="31" t="s">
-        <v>42</v>
-      </c>
-      <c r="B16" s="32" t="s">
-        <v>43</v>
-      </c>
-      <c r="C16" s="33"/>
-      <c r="D16" s="33"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G16" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H16" s="35" t="s">
-        <v>21</v>
-      </c>
+      <c r="A16" s="22"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="25"/>
+      <c r="G16" s="25"/>
+      <c r="H16" s="25"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="41"/>
-      <c r="K16" s="45"/>
-      <c r="L16" s="46"/>
-      <c r="M16" s="41"/>
+      <c r="J16" s="35"/>
+      <c r="K16" s="39"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="35"/>
     </row>
     <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A17" s="31" t="s">
-        <v>44</v>
-      </c>
-      <c r="B17" s="32" t="s">
-        <v>45</v>
-      </c>
-      <c r="C17" s="33"/>
-      <c r="D17" s="33"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H17" s="35" t="s">
-        <v>21</v>
-      </c>
+      <c r="A17" s="22"/>
+      <c r="B17" s="23"/>
+      <c r="C17" s="24"/>
+      <c r="D17" s="24"/>
+      <c r="E17" s="23"/>
+      <c r="F17" s="25"/>
+      <c r="G17" s="25"/>
+      <c r="H17" s="25"/>
       <c r="I17" s="23"/>
-      <c r="J17" s="41"/>
-      <c r="K17" s="45"/>
-      <c r="L17" s="46"/>
-      <c r="M17" s="41"/>
+      <c r="J17" s="35"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="35"/>
     </row>
     <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A18" s="31" t="s">
-        <v>46</v>
-      </c>
-      <c r="B18" s="32" t="s">
-        <v>47</v>
-      </c>
-      <c r="C18" s="33"/>
-      <c r="D18" s="33"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="34" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" s="35" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" s="35" t="s">
-        <v>21</v>
-      </c>
+      <c r="A18" s="22"/>
+      <c r="B18" s="23"/>
+      <c r="C18" s="24"/>
+      <c r="D18" s="24"/>
+      <c r="E18" s="23"/>
+      <c r="F18" s="25"/>
+      <c r="G18" s="25"/>
+      <c r="H18" s="25"/>
       <c r="I18" s="23"/>
-      <c r="J18" s="41"/>
-      <c r="K18" s="45"/>
-      <c r="L18" s="46"/>
-      <c r="M18" s="41"/>
+      <c r="J18" s="35"/>
+      <c r="K18" s="39"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="35"/>
     </row>
     <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A19" s="22"/>
@@ -2057,10 +1834,10 @@
       <c r="G19" s="25"/>
       <c r="H19" s="25"/>
       <c r="I19" s="23"/>
-      <c r="J19" s="41"/>
-      <c r="K19" s="45"/>
-      <c r="L19" s="46"/>
-      <c r="M19" s="41"/>
+      <c r="J19" s="35"/>
+      <c r="K19" s="39"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="35"/>
     </row>
     <row r="20" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A20" s="22"/>
@@ -2072,10 +1849,10 @@
       <c r="G20" s="25"/>
       <c r="H20" s="25"/>
       <c r="I20" s="23"/>
-      <c r="J20" s="41"/>
-      <c r="K20" s="45"/>
-      <c r="L20" s="46"/>
-      <c r="M20" s="41"/>
+      <c r="J20" s="35"/>
+      <c r="K20" s="39"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="35"/>
     </row>
     <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A21" s="22"/>
@@ -2087,10 +1864,10 @@
       <c r="G21" s="25"/>
       <c r="H21" s="25"/>
       <c r="I21" s="23"/>
-      <c r="J21" s="41"/>
-      <c r="K21" s="45"/>
-      <c r="L21" s="46"/>
-      <c r="M21" s="41"/>
+      <c r="J21" s="35"/>
+      <c r="K21" s="39"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="35"/>
     </row>
     <row r="22" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A22" s="22"/>
@@ -2102,10 +1879,10 @@
       <c r="G22" s="25"/>
       <c r="H22" s="25"/>
       <c r="I22" s="23"/>
-      <c r="J22" s="41"/>
-      <c r="K22" s="45"/>
-      <c r="L22" s="46"/>
-      <c r="M22" s="41"/>
+      <c r="J22" s="35"/>
+      <c r="K22" s="39"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="35"/>
     </row>
     <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A23" s="22"/>
@@ -2117,10 +1894,10 @@
       <c r="G23" s="25"/>
       <c r="H23" s="25"/>
       <c r="I23" s="23"/>
-      <c r="J23" s="41"/>
-      <c r="K23" s="45"/>
-      <c r="L23" s="46"/>
-      <c r="M23" s="41"/>
+      <c r="J23" s="35"/>
+      <c r="K23" s="39"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="35"/>
     </row>
     <row r="24" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A24" s="22"/>
@@ -2132,10 +1909,10 @@
       <c r="G24" s="25"/>
       <c r="H24" s="25"/>
       <c r="I24" s="23"/>
-      <c r="J24" s="41"/>
-      <c r="K24" s="45"/>
-      <c r="L24" s="46"/>
-      <c r="M24" s="41"/>
+      <c r="J24" s="35"/>
+      <c r="K24" s="39"/>
+      <c r="L24" s="40"/>
+      <c r="M24" s="35"/>
     </row>
     <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A25" s="22"/>
@@ -2147,10 +1924,10 @@
       <c r="G25" s="25"/>
       <c r="H25" s="25"/>
       <c r="I25" s="23"/>
-      <c r="J25" s="41"/>
-      <c r="K25" s="45"/>
-      <c r="L25" s="46"/>
-      <c r="M25" s="41"/>
+      <c r="J25" s="35"/>
+      <c r="K25" s="39"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="35"/>
     </row>
     <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A26" s="22"/>
@@ -2162,14 +1939,14 @@
       <c r="G26" s="25"/>
       <c r="H26" s="25"/>
       <c r="I26" s="23"/>
-      <c r="J26" s="41"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="46"/>
-      <c r="M26" s="41"/>
+      <c r="J26" s="35"/>
+      <c r="K26" s="39"/>
+      <c r="L26" s="40"/>
+      <c r="M26" s="35"/>
     </row>
     <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A27" s="22"/>
-      <c r="B27" s="36"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="24"/>
       <c r="D27" s="24"/>
       <c r="E27" s="23"/>
@@ -2177,10 +1954,10 @@
       <c r="G27" s="25"/>
       <c r="H27" s="25"/>
       <c r="I27" s="23"/>
-      <c r="J27" s="41"/>
-      <c r="K27" s="45"/>
-      <c r="L27" s="46"/>
-      <c r="M27" s="41"/>
+      <c r="J27" s="35"/>
+      <c r="K27" s="39"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="35"/>
     </row>
     <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A28" s="22"/>
@@ -2192,10 +1969,10 @@
       <c r="G28" s="25"/>
       <c r="H28" s="25"/>
       <c r="I28" s="23"/>
-      <c r="J28" s="41"/>
-      <c r="K28" s="45"/>
-      <c r="L28" s="46"/>
-      <c r="M28" s="41"/>
+      <c r="J28" s="35"/>
+      <c r="K28" s="39"/>
+      <c r="L28" s="40"/>
+      <c r="M28" s="35"/>
     </row>
     <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A29" s="22"/>
@@ -2207,10 +1984,10 @@
       <c r="G29" s="25"/>
       <c r="H29" s="25"/>
       <c r="I29" s="23"/>
-      <c r="J29" s="41"/>
-      <c r="K29" s="45"/>
-      <c r="L29" s="46"/>
-      <c r="M29" s="41"/>
+      <c r="J29" s="35"/>
+      <c r="K29" s="39"/>
+      <c r="L29" s="40"/>
+      <c r="M29" s="35"/>
     </row>
     <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A30" s="22"/>
@@ -2222,10 +1999,10 @@
       <c r="G30" s="25"/>
       <c r="H30" s="25"/>
       <c r="I30" s="23"/>
-      <c r="J30" s="41"/>
-      <c r="K30" s="45"/>
-      <c r="L30" s="46"/>
-      <c r="M30" s="41"/>
+      <c r="J30" s="35"/>
+      <c r="K30" s="39"/>
+      <c r="L30" s="40"/>
+      <c r="M30" s="35"/>
     </row>
     <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A31" s="22"/>
@@ -2237,10 +2014,10 @@
       <c r="G31" s="25"/>
       <c r="H31" s="25"/>
       <c r="I31" s="23"/>
-      <c r="J31" s="41"/>
-      <c r="K31" s="45"/>
-      <c r="L31" s="46"/>
-      <c r="M31" s="41"/>
+      <c r="J31" s="35"/>
+      <c r="K31" s="39"/>
+      <c r="L31" s="40"/>
+      <c r="M31" s="35"/>
     </row>
     <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A32" s="22"/>
@@ -2252,10 +2029,10 @@
       <c r="G32" s="25"/>
       <c r="H32" s="25"/>
       <c r="I32" s="23"/>
-      <c r="J32" s="41"/>
-      <c r="K32" s="45"/>
-      <c r="L32" s="46"/>
-      <c r="M32" s="41"/>
+      <c r="J32" s="35"/>
+      <c r="K32" s="39"/>
+      <c r="L32" s="40"/>
+      <c r="M32" s="35"/>
     </row>
     <row r="33" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A33" s="22"/>
@@ -2267,10 +2044,10 @@
       <c r="G33" s="25"/>
       <c r="H33" s="25"/>
       <c r="I33" s="23"/>
-      <c r="J33" s="41"/>
-      <c r="K33" s="45"/>
-      <c r="L33" s="46"/>
-      <c r="M33" s="41"/>
+      <c r="J33" s="35"/>
+      <c r="K33" s="39"/>
+      <c r="L33" s="40"/>
+      <c r="M33" s="35"/>
     </row>
     <row r="34" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A34" s="22"/>
@@ -2282,10 +2059,10 @@
       <c r="G34" s="25"/>
       <c r="H34" s="25"/>
       <c r="I34" s="23"/>
-      <c r="J34" s="41"/>
-      <c r="K34" s="45"/>
-      <c r="L34" s="46"/>
-      <c r="M34" s="41"/>
+      <c r="J34" s="35"/>
+      <c r="K34" s="39"/>
+      <c r="L34" s="40"/>
+      <c r="M34" s="35"/>
     </row>
     <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A35" s="22"/>
@@ -2297,10 +2074,10 @@
       <c r="G35" s="25"/>
       <c r="H35" s="25"/>
       <c r="I35" s="23"/>
-      <c r="J35" s="41"/>
-      <c r="K35" s="45"/>
-      <c r="L35" s="46"/>
-      <c r="M35" s="41"/>
+      <c r="J35" s="35"/>
+      <c r="K35" s="39"/>
+      <c r="L35" s="40"/>
+      <c r="M35" s="35"/>
     </row>
     <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A36" s="22"/>
@@ -2312,10 +2089,10 @@
       <c r="G36" s="25"/>
       <c r="H36" s="25"/>
       <c r="I36" s="23"/>
-      <c r="J36" s="41"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="46"/>
-      <c r="M36" s="41"/>
+      <c r="J36" s="35"/>
+      <c r="K36" s="39"/>
+      <c r="L36" s="40"/>
+      <c r="M36" s="35"/>
     </row>
     <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A37" s="22"/>
@@ -2327,10 +2104,10 @@
       <c r="G37" s="25"/>
       <c r="H37" s="25"/>
       <c r="I37" s="23"/>
-      <c r="J37" s="41"/>
-      <c r="K37" s="45"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="41"/>
+      <c r="J37" s="35"/>
+      <c r="K37" s="39"/>
+      <c r="L37" s="40"/>
+      <c r="M37" s="35"/>
     </row>
     <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
       <c r="A38" s="22"/>
@@ -2342,175 +2119,10 @@
       <c r="G38" s="25"/>
       <c r="H38" s="25"/>
       <c r="I38" s="23"/>
-      <c r="J38" s="41"/>
-      <c r="K38" s="45"/>
-      <c r="L38" s="46"/>
-      <c r="M38" s="41"/>
-    </row>
-    <row r="39" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A39" s="22"/>
-      <c r="B39" s="23"/>
-      <c r="C39" s="24"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="25"/>
-      <c r="G39" s="25"/>
-      <c r="H39" s="25"/>
-      <c r="I39" s="23"/>
-      <c r="J39" s="41"/>
-      <c r="K39" s="45"/>
-      <c r="L39" s="46"/>
-      <c r="M39" s="41"/>
-    </row>
-    <row r="40" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A40" s="22"/>
-      <c r="B40" s="23"/>
-      <c r="C40" s="24"/>
-      <c r="D40" s="24"/>
-      <c r="E40" s="23"/>
-      <c r="F40" s="25"/>
-      <c r="G40" s="25"/>
-      <c r="H40" s="25"/>
-      <c r="I40" s="23"/>
-      <c r="J40" s="41"/>
-      <c r="K40" s="45"/>
-      <c r="L40" s="46"/>
-      <c r="M40" s="41"/>
-    </row>
-    <row r="41" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A41" s="22"/>
-      <c r="B41" s="23"/>
-      <c r="C41" s="24"/>
-      <c r="D41" s="24"/>
-      <c r="E41" s="23"/>
-      <c r="F41" s="25"/>
-      <c r="G41" s="25"/>
-      <c r="H41" s="25"/>
-      <c r="I41" s="23"/>
-      <c r="J41" s="41"/>
-      <c r="K41" s="45"/>
-      <c r="L41" s="46"/>
-      <c r="M41" s="41"/>
-    </row>
-    <row r="42" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A42" s="22"/>
-      <c r="B42" s="23"/>
-      <c r="C42" s="24"/>
-      <c r="D42" s="24"/>
-      <c r="E42" s="23"/>
-      <c r="F42" s="25"/>
-      <c r="G42" s="25"/>
-      <c r="H42" s="25"/>
-      <c r="I42" s="23"/>
-      <c r="J42" s="41"/>
-      <c r="K42" s="45"/>
-      <c r="L42" s="46"/>
-      <c r="M42" s="41"/>
-    </row>
-    <row r="43" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A43" s="22"/>
-      <c r="B43" s="23"/>
-      <c r="C43" s="24"/>
-      <c r="D43" s="24"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="25"/>
-      <c r="G43" s="25"/>
-      <c r="H43" s="25"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="41"/>
-      <c r="K43" s="45"/>
-      <c r="L43" s="46"/>
-      <c r="M43" s="41"/>
-    </row>
-    <row r="44" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A44" s="22"/>
-      <c r="B44" s="23"/>
-      <c r="C44" s="24"/>
-      <c r="D44" s="24"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="25"/>
-      <c r="G44" s="25"/>
-      <c r="H44" s="25"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="41"/>
-      <c r="K44" s="45"/>
-      <c r="L44" s="46"/>
-      <c r="M44" s="41"/>
-    </row>
-    <row r="45" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A45" s="22"/>
-      <c r="B45" s="23"/>
-      <c r="C45" s="24"/>
-      <c r="D45" s="24"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="25"/>
-      <c r="G45" s="25"/>
-      <c r="H45" s="25"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="41"/>
-      <c r="K45" s="45"/>
-      <c r="L45" s="46"/>
-      <c r="M45" s="41"/>
-    </row>
-    <row r="46" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A46" s="22"/>
-      <c r="B46" s="23"/>
-      <c r="C46" s="24"/>
-      <c r="D46" s="24"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="25"/>
-      <c r="G46" s="25"/>
-      <c r="H46" s="25"/>
-      <c r="I46" s="23"/>
-      <c r="J46" s="41"/>
-      <c r="K46" s="45"/>
-      <c r="L46" s="46"/>
-      <c r="M46" s="41"/>
-    </row>
-    <row r="47" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A47" s="22"/>
-      <c r="B47" s="23"/>
-      <c r="C47" s="24"/>
-      <c r="D47" s="24"/>
-      <c r="E47" s="23"/>
-      <c r="F47" s="25"/>
-      <c r="G47" s="25"/>
-      <c r="H47" s="25"/>
-      <c r="I47" s="23"/>
-      <c r="J47" s="41"/>
-      <c r="K47" s="45"/>
-      <c r="L47" s="46"/>
-      <c r="M47" s="41"/>
-    </row>
-    <row r="48" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A48" s="22"/>
-      <c r="B48" s="23"/>
-      <c r="C48" s="24"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="23"/>
-      <c r="F48" s="25"/>
-      <c r="G48" s="25"/>
-      <c r="H48" s="25"/>
-      <c r="I48" s="23"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="45"/>
-      <c r="L48" s="46"/>
-      <c r="M48" s="41"/>
-    </row>
-    <row r="49" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A49" s="22"/>
-      <c r="B49" s="23"/>
-      <c r="C49" s="24"/>
-      <c r="D49" s="24"/>
-      <c r="E49" s="23"/>
-      <c r="F49" s="25"/>
-      <c r="G49" s="25"/>
-      <c r="H49" s="25"/>
-      <c r="I49" s="23"/>
-      <c r="J49" s="41"/>
-      <c r="K49" s="45"/>
-      <c r="L49" s="46"/>
-      <c r="M49" s="41"/>
+      <c r="J38" s="35"/>
+      <c r="K38" s="39"/>
+      <c r="L38" s="40"/>
+      <c r="M38" s="35"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
@@ -2520,9 +2132,9 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="K2:M2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:A18">
+  <conditionalFormatting sqref="A5:A7">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
-      <formula>LEN(TRIM(A6))&gt;0</formula>
+      <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L$1:L$1048576">
@@ -2536,13 +2148,13 @@
       <formula>LEFT(L1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:M18 A5 A19:M49">
+  <conditionalFormatting sqref="A8:M38 B5:M7">
     <cfRule type="notContainsBlanks" dxfId="0" priority="12">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:H5 F15:H15 F10:F14 F16:F18 G10:G14 G16:G18 H10:H14 H16:H18 F6:H9 F19:H49">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:H5 F6 G6 H6 F7 G7 H7 F8:H38">
       <formula1>"yes, no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Chnaged the test plan to verify only gkuser is running
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -48,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
   <si>
     <t>summary</t>
   </si>
@@ -104,28 +104,16 @@
     <t>reason</t>
   </si>
   <si>
-    <t>Customer and Supplier Core API Test Suite</t>
-  </si>
-  <si>
-    <t>CustomerandSupplier</t>
+    <t>GK user suite</t>
+  </si>
+  <si>
+    <t>GKUser</t>
   </si>
   <si>
     <t>yes</t>
   </si>
   <si>
     <t>no</t>
-  </si>
-  <si>
-    <t>Product Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Product</t>
-  </si>
-  <si>
-    <t>Tax Core API Test Suite</t>
-  </si>
-  <si>
-    <t>Tax</t>
   </si>
 </sst>
 </file>
@@ -138,7 +126,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="30">
+  <fonts count="29">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -192,11 +180,6 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Tahoma"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Consolas"/>
       <charset val="134"/>
     </font>
     <font>
@@ -804,135 +787,135 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="10" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1033,14 +1016,11 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="8" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
@@ -1467,13 +1447,13 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5" outlineLevelRow="4"/>
   <cols>
     <col min="1" max="1" width="47.9" style="3" customWidth="1"/>
     <col min="2" max="2" width="25" style="4" customWidth="1"/>
@@ -1505,13 +1485,13 @@
       <c r="H1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="31"/>
-      <c r="J1" s="32"/>
+      <c r="I1" s="30"/>
+      <c r="J1" s="31"/>
       <c r="K1" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="33"/>
-      <c r="M1" s="34"/>
+      <c r="L1" s="32"/>
+      <c r="M1" s="33"/>
     </row>
     <row r="2" ht="147" customHeight="1" spans="1:13">
       <c r="A2" s="16" t="s">
@@ -1525,10 +1505,10 @@
       <c r="G2" s="20"/>
       <c r="H2" s="21"/>
       <c r="I2" s="19"/>
-      <c r="J2" s="35"/>
-      <c r="K2" s="36"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="38"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="37"/>
     </row>
     <row r="3" ht="10" customHeight="1" spans="1:13">
       <c r="A3" s="22"/>
@@ -1540,10 +1520,10 @@
       <c r="G3" s="25"/>
       <c r="H3" s="25"/>
       <c r="I3" s="23"/>
-      <c r="J3" s="35"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="40"/>
-      <c r="M3" s="35"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="38"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="34"/>
     </row>
     <row r="4" s="1" customFormat="1" ht="20" customHeight="1" spans="1:13">
       <c r="A4" s="26" t="s">
@@ -1573,8 +1553,8 @@
       <c r="I4" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="35"/>
-      <c r="K4" s="41" t="s">
+      <c r="J4" s="34"/>
+      <c r="K4" s="40" t="s">
         <v>15</v>
       </c>
       <c r="L4" s="26" t="s">
@@ -1604,525 +1584,10 @@
         <v>21</v>
       </c>
       <c r="I5" s="23"/>
-      <c r="J5" s="35"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="40"/>
-      <c r="M5" s="35"/>
-    </row>
-    <row r="6" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A6" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="23" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" s="23"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G6" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="35"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="40"/>
-      <c r="M6" s="35"/>
-    </row>
-    <row r="7" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A7" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="B7" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="29" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="25" t="s">
-        <v>20</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="I7" s="23"/>
-      <c r="J7" s="35"/>
-      <c r="K7" s="39"/>
-      <c r="L7" s="40"/>
-      <c r="M7" s="35"/>
-    </row>
-    <row r="8" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A8" s="22"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="25"/>
-      <c r="G8" s="25"/>
-      <c r="H8" s="25"/>
-      <c r="I8" s="23"/>
-      <c r="J8" s="35"/>
-      <c r="K8" s="39"/>
-      <c r="L8" s="40"/>
-      <c r="M8" s="35"/>
-    </row>
-    <row r="9" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A9" s="22"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="24"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="23"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="25"/>
-      <c r="I9" s="23"/>
-      <c r="J9" s="35"/>
-      <c r="K9" s="39"/>
-      <c r="L9" s="40"/>
-      <c r="M9" s="35"/>
-    </row>
-    <row r="10" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A10" s="22"/>
-      <c r="B10" s="23"/>
-      <c r="C10" s="24"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="23"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="23"/>
-      <c r="J10" s="35"/>
-      <c r="K10" s="39"/>
-      <c r="L10" s="40"/>
-      <c r="M10" s="35"/>
-    </row>
-    <row r="11" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A11" s="22"/>
-      <c r="B11" s="23"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="23"/>
-      <c r="F11" s="25"/>
-      <c r="G11" s="25"/>
-      <c r="H11" s="25"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="35"/>
-      <c r="K11" s="39"/>
-      <c r="L11" s="40"/>
-      <c r="M11" s="35"/>
-    </row>
-    <row r="12" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A12" s="22"/>
-      <c r="B12" s="23"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="23"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="25"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="35"/>
-      <c r="K12" s="39"/>
-      <c r="L12" s="40"/>
-      <c r="M12" s="35"/>
-    </row>
-    <row r="13" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A13" s="22"/>
-      <c r="B13" s="23"/>
-      <c r="C13" s="24"/>
-      <c r="D13" s="24"/>
-      <c r="E13" s="23"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="23"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="39"/>
-      <c r="L13" s="40"/>
-      <c r="M13" s="35"/>
-    </row>
-    <row r="14" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A14" s="22"/>
-      <c r="B14" s="23"/>
-      <c r="C14" s="24"/>
-      <c r="D14" s="24"/>
-      <c r="E14" s="23"/>
-      <c r="F14" s="25"/>
-      <c r="G14" s="25"/>
-      <c r="H14" s="25"/>
-      <c r="I14" s="23"/>
-      <c r="J14" s="35"/>
-      <c r="K14" s="39"/>
-      <c r="L14" s="40"/>
-      <c r="M14" s="35"/>
-    </row>
-    <row r="15" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A15" s="22"/>
-      <c r="B15" s="23"/>
-      <c r="C15" s="24"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="23"/>
-      <c r="F15" s="25"/>
-      <c r="G15" s="25"/>
-      <c r="H15" s="25"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="35"/>
-      <c r="K15" s="39"/>
-      <c r="L15" s="40"/>
-      <c r="M15" s="35"/>
-    </row>
-    <row r="16" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A16" s="22"/>
-      <c r="B16" s="30"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="25"/>
-      <c r="G16" s="25"/>
-      <c r="H16" s="25"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="39"/>
-      <c r="L16" s="40"/>
-      <c r="M16" s="35"/>
-    </row>
-    <row r="17" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A17" s="22"/>
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="23"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="25"/>
-      <c r="H17" s="25"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="39"/>
-      <c r="L17" s="40"/>
-      <c r="M17" s="35"/>
-    </row>
-    <row r="18" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A18" s="22"/>
-      <c r="B18" s="23"/>
-      <c r="C18" s="24"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="23"/>
-      <c r="F18" s="25"/>
-      <c r="G18" s="25"/>
-      <c r="H18" s="25"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="35"/>
-      <c r="K18" s="39"/>
-      <c r="L18" s="40"/>
-      <c r="M18" s="35"/>
-    </row>
-    <row r="19" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A19" s="22"/>
-      <c r="B19" s="23"/>
-      <c r="C19" s="24"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="23"/>
-      <c r="F19" s="25"/>
-      <c r="G19" s="25"/>
-      <c r="H19" s="25"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="35"/>
-      <c r="K19" s="39"/>
-      <c r="L19" s="40"/>
-      <c r="M19" s="35"/>
-    </row>
-    <row r="20" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A20" s="22"/>
-      <c r="B20" s="23"/>
-      <c r="C20" s="24"/>
-      <c r="D20" s="24"/>
-      <c r="E20" s="23"/>
-      <c r="F20" s="25"/>
-      <c r="G20" s="25"/>
-      <c r="H20" s="25"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="35"/>
-      <c r="K20" s="39"/>
-      <c r="L20" s="40"/>
-      <c r="M20" s="35"/>
-    </row>
-    <row r="21" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A21" s="22"/>
-      <c r="B21" s="23"/>
-      <c r="C21" s="24"/>
-      <c r="D21" s="24"/>
-      <c r="E21" s="23"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="35"/>
-      <c r="K21" s="39"/>
-      <c r="L21" s="40"/>
-      <c r="M21" s="35"/>
-    </row>
-    <row r="22" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A22" s="22"/>
-      <c r="B22" s="23"/>
-      <c r="C22" s="24"/>
-      <c r="D22" s="24"/>
-      <c r="E22" s="23"/>
-      <c r="F22" s="25"/>
-      <c r="G22" s="25"/>
-      <c r="H22" s="25"/>
-      <c r="I22" s="23"/>
-      <c r="J22" s="35"/>
-      <c r="K22" s="39"/>
-      <c r="L22" s="40"/>
-      <c r="M22" s="35"/>
-    </row>
-    <row r="23" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A23" s="22"/>
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="23"/>
-      <c r="F23" s="25"/>
-      <c r="G23" s="25"/>
-      <c r="H23" s="25"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="39"/>
-      <c r="L23" s="40"/>
-      <c r="M23" s="35"/>
-    </row>
-    <row r="24" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A24" s="22"/>
-      <c r="B24" s="23"/>
-      <c r="C24" s="24"/>
-      <c r="D24" s="24"/>
-      <c r="E24" s="23"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="25"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="35"/>
-      <c r="K24" s="39"/>
-      <c r="L24" s="40"/>
-      <c r="M24" s="35"/>
-    </row>
-    <row r="25" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A25" s="22"/>
-      <c r="B25" s="23"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="23"/>
-      <c r="F25" s="25"/>
-      <c r="G25" s="25"/>
-      <c r="H25" s="25"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="35"/>
-      <c r="K25" s="39"/>
-      <c r="L25" s="40"/>
-      <c r="M25" s="35"/>
-    </row>
-    <row r="26" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A26" s="22"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="E26" s="23"/>
-      <c r="F26" s="25"/>
-      <c r="G26" s="25"/>
-      <c r="H26" s="25"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="35"/>
-      <c r="K26" s="39"/>
-      <c r="L26" s="40"/>
-      <c r="M26" s="35"/>
-    </row>
-    <row r="27" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A27" s="22"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="E27" s="23"/>
-      <c r="F27" s="25"/>
-      <c r="G27" s="25"/>
-      <c r="H27" s="25"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="35"/>
-      <c r="K27" s="39"/>
-      <c r="L27" s="40"/>
-      <c r="M27" s="35"/>
-    </row>
-    <row r="28" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A28" s="22"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="35"/>
-      <c r="K28" s="39"/>
-      <c r="L28" s="40"/>
-      <c r="M28" s="35"/>
-    </row>
-    <row r="29" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A29" s="22"/>
-      <c r="B29" s="23"/>
-      <c r="C29" s="24"/>
-      <c r="D29" s="24"/>
-      <c r="E29" s="23"/>
-      <c r="F29" s="25"/>
-      <c r="G29" s="25"/>
-      <c r="H29" s="25"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="35"/>
-      <c r="K29" s="39"/>
-      <c r="L29" s="40"/>
-      <c r="M29" s="35"/>
-    </row>
-    <row r="30" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A30" s="22"/>
-      <c r="B30" s="23"/>
-      <c r="C30" s="24"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="23"/>
-      <c r="F30" s="25"/>
-      <c r="G30" s="25"/>
-      <c r="H30" s="25"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="35"/>
-      <c r="K30" s="39"/>
-      <c r="L30" s="40"/>
-      <c r="M30" s="35"/>
-    </row>
-    <row r="31" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A31" s="22"/>
-      <c r="B31" s="23"/>
-      <c r="C31" s="24"/>
-      <c r="D31" s="24"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="25"/>
-      <c r="G31" s="25"/>
-      <c r="H31" s="25"/>
-      <c r="I31" s="23"/>
-      <c r="J31" s="35"/>
-      <c r="K31" s="39"/>
-      <c r="L31" s="40"/>
-      <c r="M31" s="35"/>
-    </row>
-    <row r="32" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A32" s="22"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
-      <c r="D32" s="24"/>
-      <c r="E32" s="23"/>
-      <c r="F32" s="25"/>
-      <c r="G32" s="25"/>
-      <c r="H32" s="25"/>
-      <c r="I32" s="23"/>
-      <c r="J32" s="35"/>
-      <c r="K32" s="39"/>
-      <c r="L32" s="40"/>
-      <c r="M32" s="35"/>
-    </row>
-    <row r="33" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A33" s="22"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
-      <c r="D33" s="24"/>
-      <c r="E33" s="23"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="23"/>
-      <c r="J33" s="35"/>
-      <c r="K33" s="39"/>
-      <c r="L33" s="40"/>
-      <c r="M33" s="35"/>
-    </row>
-    <row r="34" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A34" s="22"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
-      <c r="D34" s="24"/>
-      <c r="E34" s="23"/>
-      <c r="F34" s="25"/>
-      <c r="G34" s="25"/>
-      <c r="H34" s="25"/>
-      <c r="I34" s="23"/>
-      <c r="J34" s="35"/>
-      <c r="K34" s="39"/>
-      <c r="L34" s="40"/>
-      <c r="M34" s="35"/>
-    </row>
-    <row r="35" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A35" s="22"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="23"/>
-      <c r="F35" s="25"/>
-      <c r="G35" s="25"/>
-      <c r="H35" s="25"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="35"/>
-      <c r="K35" s="39"/>
-      <c r="L35" s="40"/>
-      <c r="M35" s="35"/>
-    </row>
-    <row r="36" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A36" s="22"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
-      <c r="D36" s="24"/>
-      <c r="E36" s="23"/>
-      <c r="F36" s="25"/>
-      <c r="G36" s="25"/>
-      <c r="H36" s="25"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="35"/>
-      <c r="K36" s="39"/>
-      <c r="L36" s="40"/>
-      <c r="M36" s="35"/>
-    </row>
-    <row r="37" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A37" s="22"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
-      <c r="D37" s="24"/>
-      <c r="E37" s="23"/>
-      <c r="F37" s="25"/>
-      <c r="G37" s="25"/>
-      <c r="H37" s="25"/>
-      <c r="I37" s="23"/>
-      <c r="J37" s="35"/>
-      <c r="K37" s="39"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="35"/>
-    </row>
-    <row r="38" s="2" customFormat="1" ht="23" customHeight="1" spans="1:13">
-      <c r="A38" s="22"/>
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="23"/>
-      <c r="F38" s="25"/>
-      <c r="G38" s="25"/>
-      <c r="H38" s="25"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="35"/>
-      <c r="K38" s="39"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="35"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="38"/>
+      <c r="L5" s="39"/>
+      <c r="M5" s="34"/>
     </row>
   </sheetData>
   <sheetProtection insertRows="0" insertColumns="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0"/>
@@ -2132,12 +1597,17 @@
     <mergeCell ref="A2:E2"/>
     <mergeCell ref="K2:M2"/>
   </mergeCells>
-  <conditionalFormatting sqref="A5:A7">
+  <conditionalFormatting sqref="A5">
     <cfRule type="notContainsBlanks" dxfId="0" priority="1">
       <formula>LEN(TRIM(A5))&gt;0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L$1:L$1048576">
+  <conditionalFormatting sqref="B5:M5">
+    <cfRule type="notContainsBlanks" dxfId="0" priority="12">
+      <formula>LEN(TRIM(B5))&gt;0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L1:L5">
     <cfRule type="beginsWith" dxfId="1" priority="2" operator="equal" text="WARN ">
       <formula>LEFT(L1,LEN("WARN "))="WARN "</formula>
     </cfRule>
@@ -2148,13 +1618,8 @@
       <formula>LEFT(L1,LEN("PASS"))="PASS"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A8:M38 B5:M7">
-    <cfRule type="notContainsBlanks" dxfId="0" priority="12">
-      <formula>LEN(TRIM(A5))&gt;0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:H5 F6 G6 H6 F7 G7 H7 F8:H38">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5:H5">
       <formula1>"yes, no"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Added mohan's scrpt to execute on pipeline
</commit_message>
<xml_diff>
--- a/tests/artifact/plan/GNUKhata-plan.xlsx
+++ b/tests/artifact/plan/GNUKhata-plan.xlsx
@@ -104,10 +104,10 @@
     <t>reason</t>
   </si>
   <si>
-    <t>GK user suite</t>
-  </si>
-  <si>
-    <t>GKUser</t>
+    <t>Tax module should run fine on CICD</t>
+  </si>
+  <si>
+    <t>Tax</t>
   </si>
   <si>
     <t>yes</t>
@@ -1450,7 +1450,7 @@
   <dimension ref="A1:M5"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="14.5" outlineLevelRow="4"/>

</xml_diff>